<commit_message>
Updated the AR data vetting tracking spreadsheets (with DR4 updates)
</commit_message>
<xml_diff>
--- a/data/target_metadata/LMC_AR_data_tracking.xlsx
+++ b/data/target_metadata/LMC_AR_data_tracking.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duval/Documents/ULLYSES/DR3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duval/Documents/ULLYSES/DR4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F4307-E88B-7B49-9F03-C01FF3C2F660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C965C6-AB2B-CF46-A594-8DAC952AEA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16480" yWindow="1720" windowWidth="21920" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="460" windowWidth="21920" windowHeight="18560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LMC_AR_data_tracking" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="205">
   <si>
     <t>Target</t>
   </si>
@@ -127,9 +136,6 @@
     <t>VFTS 72</t>
   </si>
   <si>
-    <t>LH 99-3</t>
-  </si>
-  <si>
     <t>STIS/E140M/1425</t>
   </si>
   <si>
@@ -580,9 +586,6 @@
     <t>NGC2004 26</t>
   </si>
   <si>
-    <t>AAOmega 30Dor 368</t>
-  </si>
-  <si>
     <t>FUSE-STIS/E140M-STIS/E230M/1978</t>
   </si>
   <si>
@@ -622,10 +625,25 @@
     <t>Max S/N 7</t>
   </si>
   <si>
-    <t>AAOmega 30Dor 333</t>
-  </si>
-  <si>
     <t>15824. 16299 (G140L ran in April 21)</t>
+  </si>
+  <si>
+    <t>VTS 180</t>
+  </si>
+  <si>
+    <t>ST92 5-31</t>
+  </si>
+  <si>
+    <t>UCAC3 42-33014</t>
+  </si>
+  <si>
+    <t>VFTS 96</t>
+  </si>
+  <si>
+    <t>15629 - low S/N (&lt;5)</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R152"/>
+  <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,10 +1852,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1852,7 +1870,7 @@
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
@@ -1863,7 +1881,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1880,7 +1898,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1903,7 +1921,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1915,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -1923,7 +1941,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1940,7 +1958,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1957,7 +1975,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1980,7 +1998,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1997,7 +2015,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -2020,10 +2038,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
         <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2046,7 +2064,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -2072,7 +2090,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2092,22 +2110,22 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
         <v>49</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>50</v>
       </c>
       <c r="I27" t="s">
         <v>13</v>
@@ -2118,7 +2136,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -2138,7 +2156,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -2155,22 +2173,22 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
         <v>53</v>
-      </c>
-      <c r="C30" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>54</v>
       </c>
       <c r="H30" t="s">
         <v>29</v>
@@ -2184,7 +2202,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2204,7 +2222,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -2221,7 +2239,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -2244,10 +2262,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2270,7 +2288,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2296,10 +2314,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -2311,10 +2329,10 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I36" t="s">
         <v>19</v>
@@ -2325,7 +2343,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -2342,7 +2360,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2359,7 +2377,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -2382,10 +2400,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -2397,18 +2415,18 @@
         <v>2</v>
       </c>
       <c r="G40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2423,7 +2441,7 @@
         <v>17</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I41" t="s">
         <v>19</v>
@@ -2434,10 +2452,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -2449,15 +2467,15 @@
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -2483,7 +2501,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -2500,7 +2518,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2512,12 +2530,12 @@
         <v>4</v>
       </c>
       <c r="G45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2529,7 +2547,7 @@
         <v>3</v>
       </c>
       <c r="G46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I46" t="s">
         <v>19</v>
@@ -2540,7 +2558,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2566,7 +2584,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2586,7 +2604,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2612,7 +2630,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2627,12 +2645,12 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2658,7 +2676,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -2678,7 +2696,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2690,12 +2708,12 @@
         <v>2</v>
       </c>
       <c r="G53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2721,7 +2739,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2747,7 +2765,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2767,7 +2785,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2793,7 +2811,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2819,7 +2837,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2839,7 +2857,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2859,7 +2877,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D61">
         <v>3</v>
@@ -2882,7 +2900,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2894,12 +2912,12 @@
         <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2911,12 +2929,12 @@
         <v>2</v>
       </c>
       <c r="G63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2931,12 +2949,12 @@
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -2962,7 +2980,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2988,7 +3006,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3008,7 +3026,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3028,7 +3046,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3040,7 +3058,7 @@
         <v>3</v>
       </c>
       <c r="G69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I69" t="s">
         <v>19</v>
@@ -3051,7 +3069,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -3074,7 +3092,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3091,7 +3109,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -3106,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I72" t="s">
         <v>13</v>
@@ -3117,27 +3135,27 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="H73" t="s">
         <v>98</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="H73" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -3149,18 +3167,18 @@
         <v>4</v>
       </c>
       <c r="G74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
         <v>101</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
-        <v>102</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3177,7 +3195,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -3197,7 +3215,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -3220,7 +3238,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -3235,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I78" t="s">
         <v>13</v>
@@ -3246,7 +3264,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -3272,7 +3290,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -3298,7 +3316,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -3318,19 +3336,19 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82" t="s">
         <v>109</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>2</v>
-      </c>
-      <c r="F82">
-        <v>2</v>
-      </c>
-      <c r="G82" t="s">
-        <v>110</v>
       </c>
       <c r="H82" t="s">
         <v>12</v>
@@ -3344,27 +3362,27 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="H83" t="s">
         <v>111</v>
-      </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="H83" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -3390,7 +3408,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -3416,7 +3434,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -3431,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I86" t="s">
         <v>19</v>
@@ -3442,7 +3460,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3462,7 +3480,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3482,7 +3500,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3505,7 +3523,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -3522,7 +3540,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -3548,7 +3566,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3568,7 +3586,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -3580,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="G93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I93" t="s">
         <v>19</v>
@@ -3591,7 +3609,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -3606,7 +3624,7 @@
         <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I94" t="s">
         <v>19</v>
@@ -3617,7 +3635,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3629,7 +3647,7 @@
         <v>4</v>
       </c>
       <c r="G95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H95" t="s">
         <v>12</v>
@@ -3637,7 +3655,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -3649,7 +3667,7 @@
         <v>2</v>
       </c>
       <c r="G96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H96" t="s">
         <v>12</v>
@@ -3663,7 +3681,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -3689,7 +3707,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -3704,12 +3722,12 @@
         <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -3724,12 +3742,12 @@
         <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -3752,7 +3770,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -3772,7 +3790,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -3792,7 +3810,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -3812,7 +3830,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -3838,7 +3856,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -3858,7 +3876,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -3884,7 +3902,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -3907,7 +3925,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3930,7 +3948,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -3950,7 +3968,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D110">
         <v>2</v>
@@ -3973,19 +3991,19 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>139</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>2</v>
+      </c>
+      <c r="G111" t="s">
         <v>140</v>
-      </c>
-      <c r="D111">
-        <v>1</v>
-      </c>
-      <c r="E111">
-        <v>1</v>
-      </c>
-      <c r="F111">
-        <v>2</v>
-      </c>
-      <c r="G111" t="s">
-        <v>141</v>
       </c>
       <c r="H111" t="s">
         <v>12</v>
@@ -3993,27 +4011,27 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>141</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="H112" t="s">
         <v>142</v>
-      </c>
-      <c r="B112">
-        <v>1</v>
-      </c>
-      <c r="D112">
-        <v>0</v>
-      </c>
-      <c r="E112">
-        <v>0</v>
-      </c>
-      <c r="F112">
-        <v>0</v>
-      </c>
-      <c r="H112" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -4025,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="G113" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H113" t="s">
         <v>12</v>
@@ -4033,7 +4051,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -4045,7 +4063,7 @@
         <v>2</v>
       </c>
       <c r="G114" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H114" t="s">
         <v>12</v>
@@ -4053,24 +4071,24 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>145</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115" t="s">
         <v>146</v>
-      </c>
-      <c r="D115">
-        <v>3</v>
-      </c>
-      <c r="E115">
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <v>3</v>
-      </c>
-      <c r="G115" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -4082,29 +4100,29 @@
         <v>3</v>
       </c>
       <c r="G116" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>148</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117" t="s">
         <v>149</v>
-      </c>
-      <c r="D117">
-        <v>1</v>
-      </c>
-      <c r="E117">
-        <v>2</v>
-      </c>
-      <c r="F117">
-        <v>3</v>
-      </c>
-      <c r="G117" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D118">
         <v>2</v>
@@ -4116,7 +4134,7 @@
         <v>4</v>
       </c>
       <c r="G118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I118" t="s">
         <v>19</v>
@@ -4127,7 +4145,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D119">
         <v>4</v>
@@ -4139,12 +4157,12 @@
         <v>5</v>
       </c>
       <c r="G119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -4156,12 +4174,12 @@
         <v>4</v>
       </c>
       <c r="G120" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D121">
         <v>2</v>
@@ -4173,12 +4191,12 @@
         <v>3</v>
       </c>
       <c r="G121" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -4190,12 +4208,12 @@
         <v>4</v>
       </c>
       <c r="G122" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -4215,7 +4233,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -4235,7 +4253,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -4255,7 +4273,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -4275,7 +4293,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -4295,7 +4313,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -4315,7 +4333,7 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -4335,7 +4353,7 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D130">
         <v>6</v>
@@ -4352,13 +4370,13 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B131" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -4375,7 +4393,7 @@
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -4395,22 +4413,22 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>166</v>
+      </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="H133" t="s">
         <v>167</v>
-      </c>
-      <c r="B133">
-        <v>1</v>
-      </c>
-      <c r="D133">
-        <v>0</v>
-      </c>
-      <c r="E133">
-        <v>0</v>
-      </c>
-      <c r="F133">
-        <v>0</v>
-      </c>
-      <c r="H133" t="s">
-        <v>168</v>
       </c>
       <c r="I133" t="s">
         <v>19</v>
@@ -4421,7 +4439,7 @@
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B134">
         <v>3</v>
@@ -4436,7 +4454,7 @@
         <v>0</v>
       </c>
       <c r="H134" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q134">
         <v>116</v>
@@ -4447,7 +4465,7 @@
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -4467,7 +4485,7 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -4487,7 +4505,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -4502,12 +4520,12 @@
         <v>0</v>
       </c>
       <c r="H137" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -4522,12 +4540,12 @@
         <v>0</v>
       </c>
       <c r="H138" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B139">
         <v>3</v>
@@ -4542,18 +4560,18 @@
         <v>0</v>
       </c>
       <c r="H139" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B140">
         <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -4570,13 +4588,13 @@
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B141">
         <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -4593,13 +4611,13 @@
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B142">
         <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -4616,7 +4634,7 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B143">
         <v>3</v>
@@ -4631,12 +4649,12 @@
         <v>0</v>
       </c>
       <c r="H143" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B144">
         <v>3</v>
@@ -4651,12 +4669,12 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B145">
         <v>3</v>
@@ -4671,12 +4689,12 @@
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B146">
         <v>3</v>
@@ -4691,12 +4709,12 @@
         <v>0</v>
       </c>
       <c r="H146" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B147">
         <v>3</v>
@@ -4711,12 +4729,12 @@
         <v>0</v>
       </c>
       <c r="H147" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B148">
         <v>3</v>
@@ -4731,12 +4749,12 @@
         <v>0</v>
       </c>
       <c r="H148" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B149">
         <v>3</v>
@@ -4756,7 +4774,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B150">
         <v>3</v>
@@ -4771,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4791,12 +4809,12 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="B152">
         <v>3</v>
@@ -4811,7 +4829,30 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>202</v>
+      </c>
+      <c r="B153" t="s">
+        <v>204</v>
+      </c>
+      <c r="C153" t="s">
+        <v>203</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+      <c r="H153" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>